<commit_message>
fix bug for saving data on server restart
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -9,20 +9,35 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="162913" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="11"/>
     </font>
     <font>
       <b val="1"/>
@@ -36,12 +51,42 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -54,9 +99,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -402,92 +456,83 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>age</t>
         </is>
       </c>
+      <c r="C1" s="2" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Ayush</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>rohan</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Ayush</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>rohan</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Rohit</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>56</t>
-        </is>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>ayush</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>saurabh</t>
+        </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>rohit</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>55</t>
+          <t>45</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>saurabh</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>50</t>
         </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
parse html to find input tag
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -402,7 +402,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
@@ -448,9 +448,19 @@
           <t>Ayush</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>-20</t>
+      <c r="B4" t="n">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>pawan pritam</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>-12</t>
         </is>
       </c>
     </row>

</xml_diff>